<commit_message>
Added column meta and tranforms example notebooks plus readme links
</commit_message>
<xml_diff>
--- a/data/columns_metadata.xlsx
+++ b/data/columns_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicia.brown/repos/connect/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E57F81-051A-A04C-AC8E-BB8DB60F4BF1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E81EADB-012C-5745-AB6A-C6530F3CDFCE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="440" windowWidth="28040" windowHeight="17060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>Unique Census geographic identifier</t>
   </si>
   <si>
-    <t>Censu notes on statistial exceptions that occurred for a given year, variable and geography</t>
-  </si>
-  <si>
     <t>Geography name</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>Survey year</t>
+  </si>
+  <si>
+    <t>Census notes on statistial exceptions that occurred for a given year, variable and geography</t>
   </si>
 </sst>
 </file>
@@ -965,7 +965,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,7 +999,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1027,7 +1027,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1041,7 +1041,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1055,7 +1055,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1069,7 +1069,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1083,7 +1083,7 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1097,7 +1097,7 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>